<commit_message>
local run for metrics
</commit_message>
<xml_diff>
--- a/scripts/netket/mbl/cluster/config.xlsx
+++ b/scripts/netket/mbl/cluster/config.xlsx
@@ -183,11 +183,11 @@
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.63"/>
@@ -195,7 +195,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.76"/>
   </cols>
@@ -285,7 +285,7 @@
         <v>10000</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>